<commit_message>
reformatted gbd.ICD.Map.xlsx to allow for html formatting. Otherwise much longer script to recognize grouped text patterns.
</commit_message>
<xml_diff>
--- a/myCBD/myInfo/gbd.ICD.Map.xlsx
+++ b/myCBD/myInfo/gbd.ICD.Map.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\DCDC ALL\CalREDIE\Peter\Code\CACommunityBurden\myCBD\myInfo\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="25440" windowHeight="12300"/>
   </bookViews>
@@ -11,7 +16,7 @@
     <sheet name="metaData" sheetId="3" r:id="rId2"/>
     <sheet name="notes" sheetId="4" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -26,7 +31,7 @@
     <author>Matt</author>
   </authors>
   <commentList>
-    <comment ref="C58" authorId="0">
+    <comment ref="C58" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -3776,7 +3781,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="###0.;###0."/>
   </numFmts>
@@ -4423,7 +4428,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -4458,7 +4463,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -4667,13 +4672,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S221"/>
+  <dimension ref="A1:S248"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C200" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C225" sqref="C225"/>
+      <selection pane="bottomRight" activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4755,7 +4760,7 @@
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A2" t="str">
-        <f t="shared" ref="A2" si="0">IF(I2="","",CONCATENATE(IF(E2="",CONCATENATE("...", D2,". "),IF(F2="",CONCATENATE("…...",D2,".",E2,". "),CONCATENATE("……...",D2,".",E2,".",F2,". "))),Q2))</f>
+        <f>IF(I2="","",CONCATENATE(IF(E2="",CONCATENATE("...", D2,". "),IF(F2="",CONCATENATE("......",D2,".",E2,". "),CONCATENATE(".........",D2,".",E2,".",F2,". "))),Q2))</f>
         <v>.... MISSING</v>
       </c>
       <c r="B2" s="8"/>
@@ -4783,8 +4788,8 @@
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A3" t="str">
-        <f>Q3</f>
-        <v>All CAUSES</v>
+        <f t="shared" ref="A3:A26" si="0">IF(I3="","",CONCATENATE(IF(E3="",CONCATENATE("...", D3,". "),IF(F3="",CONCATENATE("......",D3,".",E3,". "),CONCATENATE(".........",D3,".",E3,".",F3,". "))),Q3))</f>
+        <v>...0. All CAUSES</v>
       </c>
       <c r="B3" s="2">
         <v>0</v>
@@ -4820,7 +4825,7 @@
     </row>
     <row r="4" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" t="str">
-        <f>IF(I4="","",CONCATENATE(IF(E4="",CONCATENATE("...", D4,". "),IF(F4="",CONCATENATE("…...",D4,".",E4,". "),CONCATENATE("……...",D4,".",E4,".",F4,". "))),Q4))</f>
+        <f t="shared" si="0"/>
         <v>...A. Communicable, maternal, perinatal and nutritional conditions</v>
       </c>
       <c r="B4" s="2">
@@ -4865,8 +4870,8 @@
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A5" t="str">
-        <f t="shared" ref="A5:A68" si="1">IF(I5="","",CONCATENATE(IF(E5="",CONCATENATE("...", D5,". "),IF(F5="",CONCATENATE("…...",D5,".",E5,". "),CONCATENATE("……...",D5,".",E5,".",F5,". "))),Q5))</f>
-        <v>…...A.99. Other Infectious Diseases</v>
+        <f t="shared" si="0"/>
+        <v>......A.99. Other Infectious Diseases</v>
       </c>
       <c r="B5" s="2"/>
       <c r="C5" s="3" t="s">
@@ -4900,7 +4905,7 @@
     </row>
     <row r="6" spans="1:19" ht="27" x14ac:dyDescent="0.25">
       <c r="A6" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="B6" s="2">
@@ -4942,8 +4947,8 @@
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A7" t="str">
-        <f t="shared" si="1"/>
-        <v>…...A.01. Tuberculosis</v>
+        <f t="shared" si="0"/>
+        <v>......A.01. Tuberculosis</v>
       </c>
       <c r="B7" s="2">
         <v>3</v>
@@ -4992,8 +4997,8 @@
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A8" t="str">
-        <f t="shared" si="1"/>
-        <v>…...A.02. HIV/ and other Sexually transmitted diseases (STDs)</v>
+        <f t="shared" si="0"/>
+        <v>......A.02. HIV/ and other Sexually transmitted diseases (STDs)</v>
       </c>
       <c r="B8" s="2"/>
       <c r="C8" s="66" t="s">
@@ -5027,8 +5032,8 @@
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A9" t="str">
-        <f t="shared" si="1"/>
-        <v>……...A.02.a. Sexually transmitted diseases (STDs) excluding HIV</v>
+        <f t="shared" si="0"/>
+        <v>.........A.02.a. Sexually transmitted diseases (STDs) excluding HIV</v>
       </c>
       <c r="B9" s="2">
         <v>4</v>
@@ -5078,7 +5083,7 @@
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A10" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="B10" s="2">
@@ -5127,7 +5132,7 @@
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A11" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="B11" s="2">
@@ -5176,7 +5181,7 @@
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A12" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="B12" s="2">
@@ -5225,7 +5230,7 @@
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A13" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="B13" s="2">
@@ -5272,7 +5277,7 @@
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A14" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="B14" s="2">
@@ -5321,8 +5326,8 @@
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A15" t="str">
-        <f t="shared" si="1"/>
-        <v>……...A.02.b. HIV/AIDS</v>
+        <f t="shared" si="0"/>
+        <v>.........A.02.b. HIV/AIDS</v>
       </c>
       <c r="B15" s="2">
         <v>10</v>
@@ -5372,7 +5377,7 @@
     </row>
     <row r="16" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A16" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="B16" s="2">
@@ -5417,7 +5422,7 @@
     </row>
     <row r="17" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A17" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="B17" s="2">
@@ -5466,7 +5471,7 @@
     </row>
     <row r="18" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A18" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="B18" s="2">
@@ -5513,7 +5518,7 @@
     </row>
     <row r="19" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A19" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="B19" s="2">
@@ -5552,7 +5557,7 @@
     </row>
     <row r="20" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A20" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="B20" s="2">
@@ -5570,7 +5575,7 @@
       <c r="F20" s="1"/>
       <c r="G20" s="1"/>
       <c r="H20" s="42" t="str">
-        <f t="shared" ref="H20:H25" si="2">CONCATENATE("c",D20,E20,F20)</f>
+        <f t="shared" ref="H20:H25" si="1">CONCATENATE("c",D20,E20,F20)</f>
         <v>cA99</v>
       </c>
       <c r="I20" s="42"/>
@@ -5599,7 +5604,7 @@
     </row>
     <row r="21" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A21" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="B21" s="2">
@@ -5617,7 +5622,7 @@
       <c r="F21" s="1"/>
       <c r="G21" s="1"/>
       <c r="H21" s="42" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>cA99</v>
       </c>
       <c r="I21" s="42"/>
@@ -5646,7 +5651,7 @@
     </row>
     <row r="22" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A22" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="B22" s="2">
@@ -5664,7 +5669,7 @@
       <c r="F22" s="1"/>
       <c r="G22" s="1"/>
       <c r="H22" s="42" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>cA99</v>
       </c>
       <c r="I22" s="42"/>
@@ -5693,7 +5698,7 @@
     </row>
     <row r="23" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A23" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="B23" s="2">
@@ -5711,7 +5716,7 @@
       <c r="F23" s="1"/>
       <c r="G23" s="1"/>
       <c r="H23" s="42" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>cA99</v>
       </c>
       <c r="I23" s="42"/>
@@ -5740,8 +5745,8 @@
     </row>
     <row r="24" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A24" t="str">
-        <f t="shared" si="1"/>
-        <v>…...A.04. Meningitis</v>
+        <f t="shared" si="0"/>
+        <v>......A.04. Meningitis</v>
       </c>
       <c r="B24" s="2">
         <v>19</v>
@@ -5758,7 +5763,7 @@
       <c r="F24" s="1"/>
       <c r="G24" s="1"/>
       <c r="H24" s="42" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>cA04</v>
       </c>
       <c r="I24" s="42" t="str">
@@ -5790,8 +5795,8 @@
     </row>
     <row r="25" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A25" t="str">
-        <f t="shared" si="1"/>
-        <v>…...A.05. Encephalitis</v>
+        <f t="shared" si="0"/>
+        <v>......A.05. Encephalitis</v>
       </c>
       <c r="B25" s="2">
         <v>20</v>
@@ -5808,7 +5813,7 @@
       <c r="F25" s="1"/>
       <c r="G25" s="1"/>
       <c r="H25" s="42" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>cA05</v>
       </c>
       <c r="I25" s="42" t="str">
@@ -5840,8 +5845,8 @@
     </row>
     <row r="26" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A26" t="str">
-        <f t="shared" si="1"/>
-        <v>…...A.06. Hepatitis</v>
+        <f t="shared" si="0"/>
+        <v>......A.06. Hepatitis</v>
       </c>
       <c r="B26" s="2">
         <v>21</v>
@@ -5883,7 +5888,7 @@
     </row>
     <row r="27" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A27" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" ref="A10:A73" si="2">IF(I27="","",CONCATENATE(IF(E27="",CONCATENATE("...", D27,". "),IF(F27="",CONCATENATE("......",D27,".",E27,". "),CONCATENATE(".........",D27,".",E27,".",F27,". "))),Q27))</f>
         <v/>
       </c>
       <c r="B27" s="2">
@@ -5926,8 +5931,8 @@
     </row>
     <row r="28" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A28" t="str">
-        <f t="shared" si="1"/>
-        <v>……...A.06.a. Acute hepatitis B</v>
+        <f t="shared" si="2"/>
+        <v>.........A.06.a. Acute hepatitis B</v>
       </c>
       <c r="B28" s="2">
         <v>23</v>
@@ -5974,7 +5979,7 @@
     </row>
     <row r="29" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A29" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="B29" s="2"/>
@@ -6000,8 +6005,8 @@
     </row>
     <row r="30" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A30" t="str">
-        <f t="shared" si="1"/>
-        <v>……...A.06.b. Acute hepatitis C</v>
+        <f t="shared" si="2"/>
+        <v>.........A.06.b. Acute hepatitis C</v>
       </c>
       <c r="B30" s="2">
         <v>24</v>
@@ -6048,7 +6053,7 @@
     </row>
     <row r="31" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A31" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="B31" s="2">
@@ -6091,7 +6096,7 @@
     </row>
     <row r="32" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A32" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="B32" s="2">
@@ -6129,7 +6134,7 @@
     </row>
     <row r="33" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A33" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="B33" s="2">
@@ -6176,7 +6181,7 @@
     </row>
     <row r="34" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A34" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="B34" s="2">
@@ -6223,7 +6228,7 @@
     </row>
     <row r="35" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A35" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="B35" s="2">
@@ -6270,7 +6275,7 @@
     </row>
     <row r="36" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A36" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="B36" s="2">
@@ -6317,7 +6322,7 @@
     </row>
     <row r="37" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A37" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="B37" s="2">
@@ -6364,7 +6369,7 @@
     </row>
     <row r="38" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A38" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="B38" s="2">
@@ -6407,7 +6412,7 @@
     </row>
     <row r="39" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A39" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="B39" s="2">
@@ -6450,7 +6455,7 @@
     </row>
     <row r="40" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A40" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="B40" s="2">
@@ -6497,7 +6502,7 @@
     </row>
     <row r="41" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A41" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="B41" s="2">
@@ -6544,7 +6549,7 @@
     </row>
     <row r="42" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A42" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="B42" s="2">
@@ -6587,7 +6592,7 @@
     </row>
     <row r="43" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A43" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="B43" s="2">
@@ -6634,7 +6639,7 @@
     </row>
     <row r="44" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A44" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="B44" s="2">
@@ -6677,7 +6682,7 @@
     </row>
     <row r="45" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A45" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="B45" s="2">
@@ -6724,7 +6729,7 @@
     </row>
     <row r="46" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A46" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="B46" s="2">
@@ -6771,7 +6776,7 @@
     </row>
     <row r="47" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A47" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="B47" s="2">
@@ -6813,7 +6818,7 @@
     </row>
     <row r="48" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A48" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="B48" s="2">
@@ -6860,7 +6865,7 @@
     </row>
     <row r="49" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A49" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="B49" s="2">
@@ -6903,7 +6908,7 @@
     </row>
     <row r="50" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A50" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="B50" s="2">
@@ -6946,7 +6951,7 @@
     </row>
     <row r="51" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A51" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="B51" s="2">
@@ -6989,7 +6994,7 @@
     </row>
     <row r="52" spans="1:19" ht="20.25" x14ac:dyDescent="0.25">
       <c r="A52" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="B52" s="2">
@@ -7036,8 +7041,8 @@
     </row>
     <row r="53" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A53" t="str">
-        <f t="shared" si="1"/>
-        <v>…...A.07. Respiratory infections</v>
+        <f t="shared" si="2"/>
+        <v>......A.07. Respiratory infections</v>
       </c>
       <c r="B53" s="2">
         <v>47</v>
@@ -7083,7 +7088,7 @@
     </row>
     <row r="54" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A54" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="B54" s="2">
@@ -7130,7 +7135,7 @@
     </row>
     <row r="55" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A55" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="B55" s="2">
@@ -7177,7 +7182,7 @@
     </row>
     <row r="56" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A56" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="B56" s="2">
@@ -7224,8 +7229,8 @@
     </row>
     <row r="57" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A57" t="str">
-        <f t="shared" si="1"/>
-        <v>…...A.08. Maternal conditions</v>
+        <f t="shared" si="2"/>
+        <v>......A.08. Maternal conditions</v>
       </c>
       <c r="B57" s="2">
         <v>51</v>
@@ -7273,7 +7278,7 @@
     </row>
     <row r="58" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A58" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="B58" s="2">
@@ -7320,7 +7325,7 @@
     </row>
     <row r="59" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A59" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="B59" s="2">
@@ -7367,7 +7372,7 @@
     </row>
     <row r="60" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A60" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="B60" s="2">
@@ -7414,7 +7419,7 @@
     </row>
     <row r="61" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A61" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="B61" s="2">
@@ -7461,7 +7466,7 @@
     </row>
     <row r="62" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A62" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="B62" s="2">
@@ -7508,7 +7513,7 @@
     </row>
     <row r="63" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A63" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="B63" s="2">
@@ -7555,8 +7560,8 @@
     </row>
     <row r="64" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A64" t="str">
-        <f t="shared" si="1"/>
-        <v>…...A.09. Neonatal conditions</v>
+        <f t="shared" si="2"/>
+        <v>......A.09. Neonatal conditions</v>
       </c>
       <c r="B64" s="2">
         <v>58</v>
@@ -7604,7 +7609,7 @@
     </row>
     <row r="65" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A65" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="B65" s="2">
@@ -7651,7 +7656,7 @@
     </row>
     <row r="66" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A66" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="B66" s="2">
@@ -7698,7 +7703,7 @@
     </row>
     <row r="67" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A67" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="B67" s="2">
@@ -7745,7 +7750,7 @@
     </row>
     <row r="68" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A68" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="B68" s="2">
@@ -7792,7 +7797,7 @@
     </row>
     <row r="69" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A69" t="str">
-        <f t="shared" ref="A69:A132" si="5">IF(I69="","",CONCATENATE(IF(E69="",CONCATENATE("...", D69,". "),IF(F69="",CONCATENATE("…...",D69,".",E69,". "),CONCATENATE("……...",D69,".",E69,".",F69,". "))),Q69))</f>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="B69" s="2">
@@ -7834,7 +7839,7 @@
     </row>
     <row r="70" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A70" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="B70" s="2">
@@ -7881,7 +7886,7 @@
     </row>
     <row r="71" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A71" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="B71" s="2">
@@ -7928,7 +7933,7 @@
     </row>
     <row r="72" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A72" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="B72" s="2">
@@ -7971,7 +7976,7 @@
     </row>
     <row r="73" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A73" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="B73" s="2">
@@ -8018,7 +8023,7 @@
     </row>
     <row r="74" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A74" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" ref="A74:A137" si="5">IF(I74="","",CONCATENATE(IF(E74="",CONCATENATE("...", D74,". "),IF(F74="",CONCATENATE("......",D74,".",E74,". "),CONCATENATE(".........",D74,".",E74,".",F74,". "))),Q74))</f>
         <v/>
       </c>
       <c r="B74" s="2">
@@ -8183,7 +8188,7 @@
     <row r="78" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A78" t="str">
         <f t="shared" si="5"/>
-        <v>…...B.01. Mouth and oropharynx cancers</v>
+        <v>......B.01. Mouth and oropharynx cancers</v>
       </c>
       <c r="B78" s="2">
         <v>71</v>
@@ -8367,7 +8372,7 @@
     <row r="82" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A82" t="str">
         <f t="shared" si="5"/>
-        <v>…...B.02. Oesophagus cancer</v>
+        <v>......B.02. Oesophagus cancer</v>
       </c>
       <c r="B82" s="2">
         <v>75</v>
@@ -8417,7 +8422,7 @@
     <row r="83" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A83" t="str">
         <f t="shared" si="5"/>
-        <v>…...B.03. Stomach cancer</v>
+        <v>......B.03. Stomach cancer</v>
       </c>
       <c r="B83" s="2">
         <v>76</v>
@@ -8469,7 +8474,7 @@
     <row r="84" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A84" t="str">
         <f t="shared" si="5"/>
-        <v>…...B.04. Colon and rectum cancers</v>
+        <v>......B.04. Colon and rectum cancers</v>
       </c>
       <c r="B84" s="2">
         <v>77</v>
@@ -8519,7 +8524,7 @@
     <row r="85" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A85" t="str">
         <f t="shared" si="5"/>
-        <v>…...B.05. Liver cancer</v>
+        <v>......B.05. Liver cancer</v>
       </c>
       <c r="B85" s="2">
         <v>78</v>
@@ -8569,7 +8574,7 @@
     <row r="86" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A86" t="str">
         <f t="shared" si="5"/>
-        <v>…...B.06. Pancreas cancer</v>
+        <v>......B.06. Pancreas cancer</v>
       </c>
       <c r="B86" s="2">
         <v>79</v>
@@ -8619,7 +8624,7 @@
     <row r="87" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A87" t="str">
         <f t="shared" si="5"/>
-        <v>…...B.07. Trachea, bronchus and lung cancers</v>
+        <v>......B.07. Trachea, bronchus and lung cancers</v>
       </c>
       <c r="B87" s="2">
         <v>80</v>
@@ -8669,7 +8674,7 @@
     <row r="88" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A88" t="str">
         <f t="shared" si="5"/>
-        <v>…...B.08. Melanoma and other skin cancers</v>
+        <v>......B.08. Melanoma and other skin cancers</v>
       </c>
       <c r="B88" s="2">
         <v>81</v>
@@ -8808,7 +8813,7 @@
     <row r="91" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A91" t="str">
         <f t="shared" si="5"/>
-        <v>…...B.09. Breast cancer</v>
+        <v>......B.09. Breast cancer</v>
       </c>
       <c r="B91" s="2">
         <v>84</v>
@@ -8858,7 +8863,7 @@
     <row r="92" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A92" t="str">
         <f t="shared" si="5"/>
-        <v>…...B.10. uteri cancer</v>
+        <v>......B.10. uteri cancer</v>
       </c>
       <c r="B92" s="2"/>
       <c r="C92" s="74" t="s">
@@ -8987,7 +8992,7 @@
     <row r="95" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A95" t="str">
         <f t="shared" si="5"/>
-        <v>…...B.11. Ovary cancer</v>
+        <v>......B.11. Ovary cancer</v>
       </c>
       <c r="B95" s="2">
         <v>87</v>
@@ -9037,7 +9042,7 @@
     <row r="96" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A96" t="str">
         <f t="shared" si="5"/>
-        <v>…...B.12. Prostate cancer</v>
+        <v>......B.12. Prostate cancer</v>
       </c>
       <c r="B96" s="2">
         <v>88</v>
@@ -9134,7 +9139,7 @@
     <row r="98" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A98" t="str">
         <f t="shared" si="5"/>
-        <v>…...B.13. Kidney, renal pelvis and ureter cancer</v>
+        <v>......B.13. Kidney, renal pelvis and ureter cancer</v>
       </c>
       <c r="B98" s="2">
         <v>90</v>
@@ -9184,7 +9189,7 @@
     <row r="99" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A99" t="str">
         <f t="shared" si="5"/>
-        <v>…...B.14. Bladder cancer</v>
+        <v>......B.14. Bladder cancer</v>
       </c>
       <c r="B99" s="2">
         <v>91</v>
@@ -9234,7 +9239,7 @@
     <row r="100" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A100" t="str">
         <f t="shared" si="5"/>
-        <v>…...B.15. Brain and nervous system cancers</v>
+        <v>......B.15. Brain and nervous system cancers</v>
       </c>
       <c r="B100" s="2">
         <v>92</v>
@@ -9472,7 +9477,7 @@
     <row r="105" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A105" t="str">
         <f t="shared" si="5"/>
-        <v>…...B.16. Lymphomas and multiple myeloma</v>
+        <v>......B.16. Lymphomas and multiple myeloma</v>
       </c>
       <c r="B105" s="2">
         <v>97</v>
@@ -9568,7 +9573,7 @@
     <row r="107" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A107" t="str">
         <f t="shared" si="5"/>
-        <v>……...B.16.b. Non-Hodgkin lymphoma</v>
+        <v>.........B.16.b. Non-Hodgkin lymphoma</v>
       </c>
       <c r="B107" s="2">
         <v>99</v>
@@ -9620,7 +9625,7 @@
     <row r="108" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A108" t="str">
         <f t="shared" si="5"/>
-        <v>……...B.16.c. Multiple myeloma</v>
+        <v>.........B.16.c. Multiple myeloma</v>
       </c>
       <c r="B108" s="2">
         <v>100</v>
@@ -9672,7 +9677,7 @@
     <row r="109" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A109" t="str">
         <f t="shared" si="5"/>
-        <v>…...B.17. Leukaemia</v>
+        <v>......B.17. Leukaemia</v>
       </c>
       <c r="B109" s="2">
         <v>101</v>
@@ -9722,7 +9727,7 @@
     <row r="110" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A110" t="str">
         <f t="shared" si="5"/>
-        <v>…...B.99. Other malignant neoplasms</v>
+        <v>......B.99. Other malignant neoplasms</v>
       </c>
       <c r="B110" s="2">
         <v>102</v>
@@ -9815,7 +9820,7 @@
     <row r="112" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A112" t="str">
         <f t="shared" si="5"/>
-        <v>…...D.01. Diabetes mellitus</v>
+        <v>......D.01. Diabetes mellitus</v>
       </c>
       <c r="B112" s="2">
         <v>104</v>
@@ -9865,7 +9870,7 @@
     <row r="113" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A113" t="str">
         <f t="shared" si="5"/>
-        <v>…...D.02. Endocrine, blood, immune disorders</v>
+        <v>......D.02. Endocrine, blood, immune disorders</v>
       </c>
       <c r="B113" s="2">
         <v>105</v>
@@ -10148,7 +10153,7 @@
     <row r="119" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A119" t="str">
         <f t="shared" si="5"/>
-        <v>…...D.03. Mental Health disoders (non-subsance use)</v>
+        <v>......D.03. Mental Health disoders (non-subsance use)</v>
       </c>
       <c r="B119" s="2"/>
       <c r="C119" s="64" t="s">
@@ -10185,7 +10190,7 @@
     <row r="120" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A120" t="str">
         <f t="shared" si="5"/>
-        <v>…...D.04. Substance use (Mental Health)</v>
+        <v>......D.04. Substance use (Mental Health)</v>
       </c>
       <c r="B120" s="2"/>
       <c r="C120" s="64" t="s">
@@ -10458,7 +10463,7 @@
     <row r="127" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A127" t="str">
         <f t="shared" si="5"/>
-        <v>……...D.04.a. Alcohol use disorders</v>
+        <v>.........D.04.a. Alcohol use disorders</v>
       </c>
       <c r="B127" s="2">
         <v>116</v>
@@ -10550,7 +10555,7 @@
     <row r="129" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A129" t="str">
         <f t="shared" si="5"/>
-        <v>……...D.04.b. Opioid use disorders</v>
+        <v>.........D.04.b. Opioid use disorders</v>
       </c>
       <c r="B129" s="2">
         <v>118</v>
@@ -10602,7 +10607,7 @@
     <row r="130" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A130" t="str">
         <f t="shared" si="5"/>
-        <v>……...D.04.c. Cocaine use disorders</v>
+        <v>.........D.04.c. Cocaine use disorders</v>
       </c>
       <c r="B130" s="2">
         <v>119</v>
@@ -10654,7 +10659,7 @@
     <row r="131" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A131" t="str">
         <f t="shared" si="5"/>
-        <v>……...D.04.d. Amphetamine use disorders</v>
+        <v>.........D.04.d. Amphetamine use disorders</v>
       </c>
       <c r="B131" s="2">
         <v>120</v>
@@ -10748,7 +10753,7 @@
     </row>
     <row r="133" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A133" t="str">
-        <f t="shared" ref="A133:A196" si="12">IF(I133="","",CONCATENATE(IF(E133="",CONCATENATE("...", D133,". "),IF(F133="",CONCATENATE("…...",D133,".",E133,". "),CONCATENATE("……...",D133,".",E133,".",F133,". "))),Q133))</f>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="B133" s="2">
@@ -10795,7 +10800,7 @@
     </row>
     <row r="134" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A134" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="B134" s="2">
@@ -10838,7 +10843,7 @@
     </row>
     <row r="135" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A135" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="B135" s="2">
@@ -10885,7 +10890,7 @@
     </row>
     <row r="136" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A136" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="B136" s="2">
@@ -10928,7 +10933,7 @@
     </row>
     <row r="137" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A137" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="B137" s="2">
@@ -10964,7 +10969,7 @@
     </row>
     <row r="138" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A138" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" ref="A138:A201" si="12">IF(I138="","",CONCATENATE(IF(E138="",CONCATENATE("...", D138,". "),IF(F138="",CONCATENATE("......",D138,".",E138,". "),CONCATENATE(".........",D138,".",E138,".",F138,". "))),Q138))</f>
         <v/>
       </c>
       <c r="B138" s="2">
@@ -11183,7 +11188,7 @@
     <row r="143" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A143" t="str">
         <f t="shared" si="12"/>
-        <v>…...D.05. Alzheimer’s disease and other dementias</v>
+        <v>......D.05. Alzheimer’s disease and other dementias</v>
       </c>
       <c r="B143" s="2">
         <v>132</v>
@@ -11460,7 +11465,7 @@
     <row r="149" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A149" t="str">
         <f t="shared" si="12"/>
-        <v>…...D.06. Other neurological conditions</v>
+        <v>......D.06. Other neurological conditions</v>
       </c>
       <c r="B149" s="2">
         <v>138</v>
@@ -11947,7 +11952,7 @@
     <row r="160" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A160" t="str">
         <f t="shared" si="12"/>
-        <v>…...C.01. Hypertensive heart disease</v>
+        <v>......C.01. Hypertensive heart disease</v>
       </c>
       <c r="B160" s="2">
         <v>149</v>
@@ -11997,7 +12002,7 @@
     <row r="161" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A161" t="str">
         <f t="shared" si="12"/>
-        <v>…...C.02. Ischaemic heart disease</v>
+        <v>......C.02. Ischaemic heart disease</v>
       </c>
       <c r="B161" s="2">
         <v>150</v>
@@ -12047,7 +12052,7 @@
     <row r="162" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A162" t="str">
         <f t="shared" si="12"/>
-        <v>…...C.03. Stroke</v>
+        <v>......C.03. Stroke</v>
       </c>
       <c r="B162" s="2">
         <v>151</v>
@@ -12097,7 +12102,7 @@
     <row r="163" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A163" t="str">
         <f t="shared" si="12"/>
-        <v>…...C.04. Cardiomyopathy, myocarditis, endocarditis</v>
+        <v>......C.04. Cardiomyopathy, myocarditis, endocarditis</v>
       </c>
       <c r="B163" s="2">
         <v>152</v>
@@ -12147,7 +12152,7 @@
     <row r="164" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A164" t="str">
         <f t="shared" si="12"/>
-        <v>…...C.99. Other cardiovascular diseases</v>
+        <v>......C.99. Other cardiovascular diseases</v>
       </c>
       <c r="B164" s="2">
         <v>153</v>
@@ -12241,7 +12246,7 @@
     <row r="166" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A166" t="str">
         <f t="shared" si="12"/>
-        <v>…...D.07. Chronic obstructive pulmonary disease</v>
+        <v>......D.07. Chronic obstructive pulmonary disease</v>
       </c>
       <c r="B166" s="2">
         <v>155</v>
@@ -12338,7 +12343,7 @@
     <row r="168" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A168" t="str">
         <f t="shared" si="12"/>
-        <v>…...D.08. Other respiratory diseases</v>
+        <v>......D.08. Other respiratory diseases</v>
       </c>
       <c r="B168" s="2">
         <v>157</v>
@@ -12388,7 +12393,7 @@
     <row r="169" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A169" t="str">
         <f t="shared" si="12"/>
-        <v>…...D.09. Digestive diseases</v>
+        <v>......D.09. Digestive diseases</v>
       </c>
       <c r="B169" s="2">
         <v>158</v>
@@ -12902,7 +12907,7 @@
     <row r="180" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A180" t="str">
         <f t="shared" si="12"/>
-        <v>…...D.10. Kidney diseases</v>
+        <v>......D.10. Kidney diseases</v>
       </c>
       <c r="B180" s="2">
         <v>169</v>
@@ -13639,7 +13644,7 @@
     <row r="196" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A196" t="str">
         <f t="shared" si="12"/>
-        <v>…...D.11. Congenital anomalies</v>
+        <v>......D.11. Congenital anomalies</v>
       </c>
       <c r="B196" s="2">
         <v>185</v>
@@ -13687,7 +13692,7 @@
     </row>
     <row r="197" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A197" t="str">
-        <f t="shared" ref="A197:A221" si="18">IF(I197="","",CONCATENATE(IF(E197="",CONCATENATE("...", D197,". "),IF(F197="",CONCATENATE("…...",D197,".",E197,". "),CONCATENATE("……...",D197,".",E197,".",F197,". "))),Q197))</f>
+        <f t="shared" si="12"/>
         <v/>
       </c>
       <c r="B197" s="2">
@@ -13705,7 +13710,7 @@
       <c r="F197" s="1"/>
       <c r="G197" s="1"/>
       <c r="H197" s="42" t="str">
-        <f t="shared" ref="H197:H202" si="19">CONCATENATE("c",D197,E197,F197)</f>
+        <f t="shared" ref="H197:H202" si="18">CONCATENATE("c",D197,E197,F197)</f>
         <v>cD11</v>
       </c>
       <c r="I197" s="42"/>
@@ -13734,7 +13739,7 @@
     </row>
     <row r="198" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A198" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="12"/>
         <v/>
       </c>
       <c r="B198" s="2">
@@ -13752,7 +13757,7 @@
       <c r="F198" s="1"/>
       <c r="G198" s="1"/>
       <c r="H198" s="42" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="18"/>
         <v>cD11</v>
       </c>
       <c r="I198" s="42"/>
@@ -13781,7 +13786,7 @@
     </row>
     <row r="199" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A199" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="12"/>
         <v/>
       </c>
       <c r="B199" s="2">
@@ -13799,7 +13804,7 @@
       <c r="F199" s="1"/>
       <c r="G199" s="1"/>
       <c r="H199" s="42" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="18"/>
         <v>cD11</v>
       </c>
       <c r="I199" s="42"/>
@@ -13828,7 +13833,7 @@
     </row>
     <row r="200" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A200" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="12"/>
         <v/>
       </c>
       <c r="B200" s="2">
@@ -13846,7 +13851,7 @@
       <c r="F200" s="1"/>
       <c r="G200" s="1"/>
       <c r="H200" s="42" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="18"/>
         <v>cD11</v>
       </c>
       <c r="I200" s="42"/>
@@ -13875,7 +13880,7 @@
     </row>
     <row r="201" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A201" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="12"/>
         <v/>
       </c>
       <c r="B201" s="2">
@@ -13893,7 +13898,7 @@
       <c r="F201" s="1"/>
       <c r="G201" s="1"/>
       <c r="H201" s="42" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="18"/>
         <v>cD11</v>
       </c>
       <c r="I201" s="42"/>
@@ -13922,7 +13927,7 @@
     </row>
     <row r="202" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A202" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" ref="A202:A248" si="19">IF(I202="","",CONCATENATE(IF(E202="",CONCATENATE("...", D202,". "),IF(F202="",CONCATENATE("......",D202,".",E202,". "),CONCATENATE(".........",D202,".",E202,".",F202,". "))),Q202))</f>
         <v/>
       </c>
       <c r="B202" s="2">
@@ -13940,7 +13945,7 @@
       <c r="F202" s="1"/>
       <c r="G202" s="1"/>
       <c r="H202" s="42" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="18"/>
         <v>cD11</v>
       </c>
       <c r="I202" s="42"/>
@@ -13969,7 +13974,7 @@
     </row>
     <row r="203" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A203" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v/>
       </c>
       <c r="B203" s="2">
@@ -14009,7 +14014,7 @@
     </row>
     <row r="204" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A204" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v/>
       </c>
       <c r="B204" s="2">
@@ -14052,7 +14057,7 @@
     </row>
     <row r="205" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A205" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v/>
       </c>
       <c r="B205" s="2">
@@ -14095,7 +14100,7 @@
     </row>
     <row r="206" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A206" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v/>
       </c>
       <c r="B206" s="2">
@@ -14138,7 +14143,7 @@
     </row>
     <row r="207" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A207" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v/>
       </c>
       <c r="B207" s="2">
@@ -14181,7 +14186,7 @@
     </row>
     <row r="208" spans="1:19" ht="33.75" x14ac:dyDescent="0.25">
       <c r="A208" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>...E. Injuries</v>
       </c>
       <c r="B208" s="2">
@@ -14226,8 +14231,8 @@
     </row>
     <row r="209" spans="1:19" ht="33.75" x14ac:dyDescent="0.25">
       <c r="A209" t="str">
-        <f t="shared" si="18"/>
-        <v>…...E.01. Unintentional injuries</v>
+        <f t="shared" si="19"/>
+        <v>......E.01. Unintentional injuries</v>
       </c>
       <c r="B209" s="2">
         <v>198</v>
@@ -14273,8 +14278,8 @@
     </row>
     <row r="210" spans="1:19" ht="40.5" x14ac:dyDescent="0.25">
       <c r="A210" t="str">
-        <f t="shared" si="18"/>
-        <v>……...E.01.a. Road injury</v>
+        <f t="shared" si="19"/>
+        <v>.........E.01.a. Road injury</v>
       </c>
       <c r="B210" s="2">
         <v>199</v>
@@ -14325,7 +14330,7 @@
     </row>
     <row r="211" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A211" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v/>
       </c>
       <c r="B211" s="2">
@@ -14374,8 +14379,8 @@
     </row>
     <row r="212" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A212" t="str">
-        <f t="shared" si="18"/>
-        <v>……...E.01.b. Falls</v>
+        <f t="shared" si="19"/>
+        <v>.........E.01.b. Falls</v>
       </c>
       <c r="B212" s="2">
         <v>201</v>
@@ -14426,7 +14431,7 @@
     </row>
     <row r="213" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A213" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v/>
       </c>
       <c r="B213" s="2">
@@ -14475,7 +14480,7 @@
     </row>
     <row r="214" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A214" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v/>
       </c>
       <c r="B214" s="2">
@@ -14524,7 +14529,7 @@
     </row>
     <row r="215" spans="1:19" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A215" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v/>
       </c>
       <c r="B215" s="2">
@@ -14573,7 +14578,7 @@
     </row>
     <row r="216" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A216" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v/>
       </c>
       <c r="B216" s="2">
@@ -14618,8 +14623,8 @@
     </row>
     <row r="217" spans="1:19" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A217" t="str">
-        <f t="shared" si="18"/>
-        <v>……...E.01.x. Other unintentional injuries</v>
+        <f t="shared" si="19"/>
+        <v>.........E.01.x. Other unintentional injuries</v>
       </c>
       <c r="B217" s="2">
         <v>206</v>
@@ -14670,7 +14675,7 @@
     </row>
     <row r="218" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A218" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v/>
       </c>
       <c r="B218" s="2">
@@ -14714,8 +14719,8 @@
     </row>
     <row r="219" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A219" t="str">
-        <f t="shared" si="18"/>
-        <v>…...E.02. Suicide/Self-harm</v>
+        <f t="shared" si="19"/>
+        <v>......E.02. Suicide/Self-harm</v>
       </c>
       <c r="B219" s="2">
         <v>208</v>
@@ -14764,8 +14769,8 @@
     </row>
     <row r="220" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A220" t="str">
-        <f t="shared" si="18"/>
-        <v>…...E.03. Homicide/Interpersonal violence</v>
+        <f t="shared" si="19"/>
+        <v>......E.03. Homicide/Interpersonal violence</v>
       </c>
       <c r="B220" s="2">
         <v>209</v>
@@ -14814,7 +14819,7 @@
     </row>
     <row r="221" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A221" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v/>
       </c>
       <c r="B221" s="2">
@@ -14854,6 +14859,168 @@
         <v>142</v>
       </c>
       <c r="S221" s="2"/>
+    </row>
+    <row r="222" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A222" t="str">
+        <f t="shared" si="19"/>
+        <v/>
+      </c>
+    </row>
+    <row r="223" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A223" t="str">
+        <f t="shared" si="19"/>
+        <v/>
+      </c>
+    </row>
+    <row r="224" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A224" t="str">
+        <f t="shared" si="19"/>
+        <v/>
+      </c>
+    </row>
+    <row r="225" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A225" t="str">
+        <f t="shared" si="19"/>
+        <v/>
+      </c>
+    </row>
+    <row r="226" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A226" t="str">
+        <f t="shared" si="19"/>
+        <v/>
+      </c>
+    </row>
+    <row r="227" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A227" t="str">
+        <f t="shared" si="19"/>
+        <v/>
+      </c>
+    </row>
+    <row r="228" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A228" t="str">
+        <f t="shared" si="19"/>
+        <v/>
+      </c>
+    </row>
+    <row r="229" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A229" t="str">
+        <f t="shared" si="19"/>
+        <v/>
+      </c>
+    </row>
+    <row r="230" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A230" t="str">
+        <f t="shared" si="19"/>
+        <v/>
+      </c>
+    </row>
+    <row r="231" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A231" t="str">
+        <f t="shared" si="19"/>
+        <v/>
+      </c>
+    </row>
+    <row r="232" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A232" t="str">
+        <f t="shared" si="19"/>
+        <v/>
+      </c>
+    </row>
+    <row r="233" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A233" t="str">
+        <f t="shared" si="19"/>
+        <v/>
+      </c>
+    </row>
+    <row r="234" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A234" t="str">
+        <f t="shared" si="19"/>
+        <v/>
+      </c>
+    </row>
+    <row r="235" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A235" t="str">
+        <f t="shared" si="19"/>
+        <v/>
+      </c>
+    </row>
+    <row r="236" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A236" t="str">
+        <f t="shared" si="19"/>
+        <v/>
+      </c>
+    </row>
+    <row r="237" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A237" t="str">
+        <f t="shared" si="19"/>
+        <v/>
+      </c>
+    </row>
+    <row r="238" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A238" t="str">
+        <f t="shared" si="19"/>
+        <v/>
+      </c>
+    </row>
+    <row r="239" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A239" t="str">
+        <f t="shared" si="19"/>
+        <v/>
+      </c>
+    </row>
+    <row r="240" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A240" t="str">
+        <f t="shared" si="19"/>
+        <v/>
+      </c>
+    </row>
+    <row r="241" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A241" t="str">
+        <f t="shared" si="19"/>
+        <v/>
+      </c>
+    </row>
+    <row r="242" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A242" t="str">
+        <f t="shared" si="19"/>
+        <v/>
+      </c>
+    </row>
+    <row r="243" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A243" t="str">
+        <f t="shared" si="19"/>
+        <v/>
+      </c>
+    </row>
+    <row r="244" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A244" t="str">
+        <f t="shared" si="19"/>
+        <v/>
+      </c>
+    </row>
+    <row r="245" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A245" t="str">
+        <f t="shared" si="19"/>
+        <v/>
+      </c>
+    </row>
+    <row r="246" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A246" t="str">
+        <f t="shared" si="19"/>
+        <v/>
+      </c>
+    </row>
+    <row r="247" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A247" t="str">
+        <f t="shared" si="19"/>
+        <v/>
+      </c>
+    </row>
+    <row r="248" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A248" t="str">
+        <f t="shared" si="19"/>
+        <v/>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
trying to replace the gbd.icd file most importantly
</commit_message>
<xml_diff>
--- a/myCBD/myInfo/gbd.ICD.Map.xlsx
+++ b/myCBD/myInfo/gbd.ICD.Map.xlsx
@@ -4678,7 +4678,7 @@
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A6" sqref="A6"/>
+      <selection pane="bottomRight" activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4760,8 +4760,8 @@
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A2" t="str">
-        <f>IF(I2="","",CONCATENATE(IF(E2="",CONCATENATE("...", D2,". "),IF(F2="",CONCATENATE("......",D2,".",E2,". "),CONCATENATE(".........",D2,".",E2,".",F2,". "))),Q2))</f>
-        <v>.... MISSING</v>
+        <f>IF(I2="","",CONCATENATE(IF(E2="",CONCATENATE("...", D2,"."),IF(F2="",CONCATENATE("......",D2,".",E2,". "),CONCATENATE(".........",D2,".",E2,".",F2,". "))),Q2))</f>
+        <v>....MISSING</v>
       </c>
       <c r="B2" s="8"/>
       <c r="C2" s="1"/>
@@ -5888,7 +5888,7 @@
     </row>
     <row r="27" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A27" t="str">
-        <f t="shared" ref="A10:A73" si="2">IF(I27="","",CONCATENATE(IF(E27="",CONCATENATE("...", D27,". "),IF(F27="",CONCATENATE("......",D27,".",E27,". "),CONCATENATE(".........",D27,".",E27,".",F27,". "))),Q27))</f>
+        <f t="shared" ref="A27:A73" si="2">IF(I27="","",CONCATENATE(IF(E27="",CONCATENATE("...", D27,". "),IF(F27="",CONCATENATE("......",D27,".",E27,". "),CONCATENATE(".........",D27,".",E27,".",F27,". "))),Q27))</f>
         <v/>
       </c>
       <c r="B27" s="2">

</xml_diff>